<commit_message>
Test Protokolle und Übersichtsdatei
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/Durchgeführte Modultests/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/Durchgeführte Modultests/00_Testübersicht.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Aufgaben_Alle ( Axx )" sheetId="1" r:id="rId1"/>
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="Auswahl">'Aufgaben_Alle ( Axx )'!$AJ$4:$AJ$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$1:$K$9</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$19</definedName>
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
   <si>
     <t>SWE Projekt HFTL-APP</t>
   </si>
@@ -141,6 +141,15 @@
   </si>
   <si>
     <t>AD</t>
+  </si>
+  <si>
+    <t>Überprüfung UML Diagramm</t>
+  </si>
+  <si>
+    <t>UML</t>
+  </si>
+  <si>
+    <t>Unterlagen</t>
   </si>
 </sst>
 </file>
@@ -323,7 +332,217 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="6"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFCC66"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -694,23 +913,23 @@
   <dimension ref="A1:BE396"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="18.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.33203125" defaultRowHeight="18.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" style="11" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" style="11" customWidth="1"/>
-    <col min="4" max="5" width="14.28515625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="28.5703125" style="10" customWidth="1"/>
-    <col min="7" max="8" width="17.140625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="17.140625" style="10" customWidth="1"/>
-    <col min="10" max="10" width="17.140625" style="8" customWidth="1"/>
-    <col min="11" max="11" width="1.7109375" style="1" customWidth="1"/>
-    <col min="12" max="55" width="14.28515625" style="1"/>
-    <col min="56" max="56" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="57" max="16384" width="14.28515625" style="1"/>
+    <col min="1" max="1" width="1.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" style="11" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" style="11" customWidth="1"/>
+    <col min="4" max="5" width="14.33203125" style="8" customWidth="1"/>
+    <col min="6" max="6" width="28.5546875" style="10" customWidth="1"/>
+    <col min="7" max="8" width="17.109375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="17.109375" style="10" customWidth="1"/>
+    <col min="10" max="10" width="17.109375" style="8" customWidth="1"/>
+    <col min="11" max="11" width="1.6640625" style="1" customWidth="1"/>
+    <col min="12" max="55" width="14.33203125" style="1"/>
+    <col min="56" max="56" width="15.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="57" max="16384" width="14.33203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:57" ht="18.75" hidden="1" customHeight="1">
@@ -783,7 +1002,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:57" ht="45">
+    <row r="5" spans="1:57" ht="28.8">
       <c r="B5" s="16">
         <v>1</v>
       </c>
@@ -813,7 +1032,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:57" ht="30">
+    <row r="6" spans="1:57" ht="28.8">
       <c r="B6" s="16">
         <f>IF(C6="","",B5+1)</f>
         <v>2</v>
@@ -844,7 +1063,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:57" ht="30">
+    <row r="7" spans="1:57" ht="28.8">
       <c r="B7" s="16">
         <f t="shared" ref="B7:B70" si="0">IF(C7="","",B6+1)</f>
         <v>3</v>
@@ -875,7 +1094,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:57" ht="30">
+    <row r="8" spans="1:57" ht="28.8">
       <c r="B8" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -911,19 +1130,35 @@
       <c r="BD8" s="17"/>
       <c r="BE8" s="8"/>
     </row>
-    <row r="9" spans="1:57" ht="15">
-      <c r="B9" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
+    <row r="9" spans="1:57" ht="14.4">
+      <c r="B9" s="16">
+        <v>5</v>
+      </c>
+      <c r="C9" s="9">
+        <v>42162</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I9" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J9" s="9"/>
+        <v>gut</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="AZ9" s="1">
         <v>1</v>
       </c>
@@ -943,19 +1178,35 @@
         <v>39</v>
       </c>
     </row>
-    <row r="10" spans="1:57" ht="15">
-      <c r="B10" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C10" s="9"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+    <row r="10" spans="1:57" ht="14.4">
+      <c r="B10" s="16">
+        <v>6</v>
+      </c>
+      <c r="C10" s="9">
+        <v>42162</v>
+      </c>
+      <c r="D10" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I10" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J10" s="9"/>
+        <v>gut</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="AZ10" s="1">
         <v>2</v>
       </c>
@@ -975,19 +1226,35 @@
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="15">
-      <c r="B11" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
+    <row r="11" spans="1:57" ht="14.4">
+      <c r="B11" s="16">
+        <v>7</v>
+      </c>
+      <c r="C11" s="9">
+        <v>42163</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="I11" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J11" s="9"/>
+        <v>befriedigend</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="AZ11" s="1">
         <v>3</v>
       </c>
@@ -997,24 +1264,42 @@
       <c r="BB11" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="BC11" s="6"/>
+      <c r="BC11" s="10" t="s">
+        <v>41</v>
+      </c>
       <c r="BE11" s="8" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:57" ht="18.75" customHeight="1">
-      <c r="B12" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C12" s="9"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
+      <c r="B12" s="16">
+        <v>8</v>
+      </c>
+      <c r="C12" s="9">
+        <v>42163</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>16</v>
+      </c>
       <c r="I12" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J12" s="9"/>
+        <v>befriedigend</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="AZ12" s="1">
         <v>4</v>
       </c>
@@ -1024,24 +1309,42 @@
       <c r="BB12" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="BC12" s="6"/>
+      <c r="BC12" s="10" t="s">
+        <v>42</v>
+      </c>
       <c r="BE12" s="8" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="15">
-      <c r="B13" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="9"/>
+    <row r="13" spans="1:57" ht="14.4">
+      <c r="B13" s="16">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9">
+        <v>42163</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>17</v>
+      </c>
       <c r="I13" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J13" s="9"/>
+        <v>gut</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="AZ13" s="1">
         <v>5</v>
       </c>
@@ -1056,19 +1359,35 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="15">
-      <c r="B14" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="C14" s="9"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9"/>
+    <row r="14" spans="1:57" ht="14.4">
+      <c r="B14" s="16">
+        <v>10</v>
+      </c>
+      <c r="C14" s="9">
+        <v>42163</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>27</v>
+      </c>
       <c r="I14" s="10" t="str">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="J14" s="9"/>
+        <v>ausreichend</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>25</v>
+      </c>
       <c r="AZ14" s="1">
         <v>6</v>
       </c>
@@ -1082,7 +1401,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="15">
+    <row r="15" spans="1:57" ht="14.4">
       <c r="B15" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1099,7 +1418,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:57" ht="15">
+    <row r="16" spans="1:57" ht="14.4">
       <c r="B16" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -1116,7 +1435,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="2:10" ht="15">
+    <row r="17" spans="2:10" ht="14.4">
       <c r="B17" s="16" t="str">
         <f t="shared" si="0"/>
         <v/>
@@ -4628,18 +4947,18 @@
     <sortCondition ref="BE16"/>
   </sortState>
   <conditionalFormatting sqref="B5:J1048576">
-    <cfRule type="expression" dxfId="8" priority="9">
+    <cfRule type="expression" dxfId="29" priority="9">
       <formula>$B5&lt;&gt;""</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="8">
+    <cfRule type="expression" dxfId="28" priority="8">
       <formula>OR($I5="ungenügend",$I5="mangelhaft")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="7">
+    <cfRule type="expression" dxfId="27" priority="7">
       <formula>$J5="bestanden"</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E221">
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E220:E221">
       <formula1>$BC$8:$BC$10</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5:G396 J5:J378">
@@ -4650,6 +4969,9 @@
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D5:D394">
       <formula1>Tester</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E5:E219">
+      <formula1>$BC$8:$BC$12</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.78740157480314965" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
@@ -4668,10 +4990,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="J382" sqref="J382"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
eigene Tests in Testübersicht eingetragen
</commit_message>
<xml_diff>
--- a/Dokumentation/Testprotokolle/Durchgeführte Modultests/00_Testübersicht.xlsx
+++ b/Dokumentation/Testprotokolle/Durchgeführte Modultests/00_Testübersicht.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <definedNames>
     <definedName name="Auswahl">'Aufgaben_Alle ( Axx )'!$AJ$4:$AJ$5</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$33</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Aufgaben_Alle ( Axx )'!$A$2:$K$35</definedName>
     <definedName name="Ergebnis">'Aufgaben_Alle ( Axx )'!$BA$7:$BA$14</definedName>
     <definedName name="Tester">'Aufgaben_Alle ( Axx )'!$BE$8:$BE$16</definedName>
   </definedNames>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="48">
   <si>
     <t>SWE Projekt HFTL-APP</t>
   </si>
@@ -347,196 +347,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="30">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="6"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -867,9 +678,9 @@
   <dimension ref="A1:BE399"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.28515625" defaultRowHeight="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1884,9 +1695,18 @@
       <c r="J32" s="9"/>
     </row>
     <row r="33" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="9">
+        <v>42226</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>44</v>
       </c>
       <c r="G33" s="9"/>
       <c r="H33" s="9"/>
@@ -1897,9 +1717,18 @@
       <c r="J33" s="9"/>
     </row>
     <row r="34" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="9">
+        <v>42226</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
@@ -1910,16 +1739,21 @@
       <c r="J34" s="9"/>
     </row>
     <row r="35" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="16" t="str">
-        <f t="shared" si="0"/>
-        <v/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="9">
+        <v>42226</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>43</v>
       </c>
       <c r="G35" s="9"/>
       <c r="H35" s="9"/>
-      <c r="I35" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
       <c r="J35" s="9"/>
     </row>
     <row r="36" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -3237,7 +3071,7 @@
     </row>
     <row r="137" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B137" s="16" t="str">
-        <f t="shared" ref="B137:B200" si="4">IF(C137="","",B136+1)</f>
+        <f t="shared" ref="B137:B199" si="4">IF(C137="","",B136+1)</f>
         <v/>
       </c>
       <c r="G137" s="9"/>
@@ -5153,13 +4987,13 @@
     <sortCondition ref="BE16"/>
   </sortState>
   <conditionalFormatting sqref="B5:J1048576">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="2" priority="7">
       <formula>$J5="bestanden"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="8">
+    <cfRule type="expression" dxfId="1" priority="8">
       <formula>OR($I5="ungenügend",$I5="mangelhaft")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="9">
+    <cfRule type="expression" dxfId="0" priority="9">
       <formula>$B5&lt;&gt;""</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>